<commit_message>
menambahkan fitur upload gambar
</commit_message>
<xml_diff>
--- a/Laporan Buku Tamu.xlsx
+++ b/Laporan Buku Tamu.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>NO</t>
   </si>
@@ -41,7 +41,7 @@
     <t>2024-09-18</t>
   </si>
   <si>
-    <t>perong</t>
+    <t>peron</t>
   </si>
   <si>
     <t>kp.loji</t>
@@ -117,6 +117,78 @@
   </si>
   <si>
     <t>ngoding</t>
+  </si>
+  <si>
+    <t>2024-10-14</t>
+  </si>
+  <si>
+    <t>ival tim</t>
+  </si>
+  <si>
+    <t>08578273282</t>
+  </si>
+  <si>
+    <t>egi tim</t>
+  </si>
+  <si>
+    <t>ngomongin tim</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>tekjtasldk</t>
+  </si>
+  <si>
+    <t>skdfsdjf</t>
+  </si>
+  <si>
+    <t>dfjsadfhk</t>
+  </si>
+  <si>
+    <t>2024-10-15</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>sdfkjasdjf</t>
+  </si>
+  <si>
+    <t>ksdfakdsj</t>
+  </si>
+  <si>
+    <t>kdfkaj</t>
+  </si>
+  <si>
+    <t>kknsdflak</t>
+  </si>
+  <si>
+    <t>2024-10-17</t>
+  </si>
+  <si>
+    <t>azid</t>
+  </si>
+  <si>
+    <t>blk</t>
+  </si>
+  <si>
+    <t>ngendong</t>
+  </si>
+  <si>
+    <t>2024-10-22</t>
+  </si>
+  <si>
+    <t>bebey</t>
+  </si>
+  <si>
+    <t>gg guntur</t>
+  </si>
+  <si>
+    <t>ffsdfg</t>
+  </si>
+  <si>
+    <t>unity</t>
   </si>
 </sst>
 </file>
@@ -456,7 +528,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -602,6 +674,121 @@
         <v>33</v>
       </c>
     </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>1232131</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10">
+        <v>1242432</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11">
+        <v>66587970854</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>